<commit_message>
template style conversion done. some new functions with tags. date stamp in posts.
</commit_message>
<xml_diff>
--- a/_plan.xlsx
+++ b/_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t>Аутентификация</t>
   </si>
@@ -218,13 +218,46 @@
   </si>
   <si>
     <t>пагинация выборки тегов (общий метод вывода ленты?)</t>
+  </si>
+  <si>
+    <t>Добавить в табл users поле uniq</t>
+  </si>
+  <si>
+    <t>Добавить табл log</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>uniq</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>os</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>fromurl</t>
+  </si>
+  <si>
+    <t>разобраться в каком месте выгодней ставить db-&gt;connect</t>
+  </si>
+  <si>
+    <t>теги при создании и редактировании поста</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +284,14 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -286,13 +327,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -594,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L61"/>
+  <dimension ref="B1:M65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,12 +649,12 @@
     <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>52</v>
       </c>
@@ -627,8 +670,11 @@
       <c r="L3" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
@@ -638,7 +684,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
@@ -657,8 +703,11 @@
       <c r="L5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>43</v>
       </c>
@@ -677,8 +726,11 @@
       <c r="L6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
@@ -694,8 +746,11 @@
       <c r="L7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
@@ -708,8 +763,11 @@
       <c r="J8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>56</v>
       </c>
@@ -719,8 +777,14 @@
       <c r="I9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
@@ -730,16 +794,22 @@
       <c r="I10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>28</v>
       </c>
@@ -747,7 +817,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>46</v>
       </c>
@@ -755,7 +825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
@@ -763,7 +833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
@@ -771,7 +841,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
         <v>50</v>
       </c>
@@ -788,8 +858,11 @@
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>57</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
@@ -801,161 +874,187 @@
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>65</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="D23" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>1</v>
+      <c r="C26" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>54</v>
+      <c r="C27" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>2</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C47" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+bootstrap - index,лента +bootstrap - post +bootstrap - edit +bootstrap - input file ! +bootstrap - modal image +bootstrap - modal tags +обо мне, ссылки +userspace +администрирование юзеров +поиск
</commit_message>
<xml_diff>
--- a/_plan.xlsx
+++ b/_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
   <si>
     <t>Аутентификация</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>Контроль безопасности длина полей ввода</t>
+  </si>
+  <si>
+    <t>pages</t>
   </si>
 </sst>
 </file>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M81"/>
+  <dimension ref="B1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,12 +678,12 @@
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>49</v>
       </c>
@@ -705,8 +708,11 @@
       <c r="M3" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
@@ -716,7 +722,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
@@ -744,8 +750,11 @@
       <c r="M5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>40</v>
       </c>
@@ -773,8 +782,11 @@
       <c r="M6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>41</v>
       </c>
@@ -799,8 +811,11 @@
       <c r="M7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>42</v>
       </c>
@@ -820,7 +835,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
         <v>53</v>
       </c>
@@ -837,7 +852,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
@@ -851,7 +866,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
@@ -865,7 +880,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
@@ -876,7 +891,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
         <v>43</v>
       </c>
@@ -884,7 +899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
         <v>45</v>
       </c>
@@ -892,7 +907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
         <v>46</v>
       </c>
@@ -900,7 +915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
         <v>47</v>
       </c>
@@ -1047,19 +1062,19 @@
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="C35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D35">
-        <v>57</v>
+      <c r="D35" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="C36" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D36">
-        <v>58</v>
+      <c r="D36" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
@@ -1127,27 +1142,27 @@
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D45">
-        <v>95</v>
+      <c r="D45" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+      <c r="C46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D46">
-        <v>98</v>
+      <c r="D46" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D47">
-        <v>99</v>
+      <c r="D47" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.25">
@@ -1159,19 +1174,19 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+      <c r="C49" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D49">
-        <v>101</v>
+      <c r="D49" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+      <c r="C50" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D50">
-        <v>102</v>
+      <c r="D50" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>